<commit_message>
Update: convert unix dateformat
</commit_message>
<xml_diff>
--- a/allCovidData.xlsx
+++ b/allCovidData.xlsx
@@ -431,8 +431,10 @@
       <c r="E2" t="n">
         <v>18</v>
       </c>
-      <c r="F2" t="n">
-        <v>1585650492000</v>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:28:12</t>
+        </is>
       </c>
       <c r="G2" t="n">
         <v>40</v>
@@ -462,8 +464,10 @@
       <c r="E3" t="n">
         <v>11</v>
       </c>
-      <c r="F3" t="n">
-        <v>1585650479000</v>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G3" t="n">
         <v>41.8719</v>
@@ -493,8 +497,10 @@
       <c r="E4" t="n">
         <v>156</v>
       </c>
-      <c r="F4" t="n">
-        <v>1585650479000</v>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G4" t="n">
         <v>40.463667</v>
@@ -524,8 +530,10 @@
       <c r="E5" t="n">
         <v>4</v>
       </c>
-      <c r="F5" t="n">
-        <v>1585645805000</v>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2020-03-31 09:10:05</t>
+        </is>
       </c>
       <c r="G5" t="n">
         <v>30.5928</v>
@@ -555,8 +563,10 @@
       <c r="E6" t="n">
         <v>8</v>
       </c>
-      <c r="F6" t="n">
-        <v>1585650479000</v>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G6" t="n">
         <v>51.1657</v>
@@ -586,8 +596,10 @@
       <c r="E7" t="n">
         <v>7</v>
       </c>
-      <c r="F7" t="n">
-        <v>1585650479000</v>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G7" t="n">
         <v>46.2276</v>
@@ -617,8 +629,10 @@
       <c r="E8" t="n">
         <v>89</v>
       </c>
-      <c r="F8" t="n">
-        <v>1585650479000</v>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G8" t="n">
         <v>32.427908</v>
@@ -648,8 +662,10 @@
       <c r="E9" t="n">
         <v>17</v>
       </c>
-      <c r="F9" t="n">
-        <v>1585650479000</v>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G9" t="n">
         <v>55</v>
@@ -679,8 +695,10 @@
       <c r="E10" t="n">
         <v>16</v>
       </c>
-      <c r="F10" t="n">
-        <v>1585650479000</v>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G10" t="n">
         <v>46.8182</v>
@@ -710,8 +728,10 @@
       <c r="E11" t="n">
         <v>33</v>
       </c>
-      <c r="F11" t="n">
-        <v>1585650479000</v>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G11" t="n">
         <v>50.8333</v>
@@ -741,8 +761,10 @@
       <c r="E12" t="n">
         <v>12</v>
       </c>
-      <c r="F12" t="n">
-        <v>1585650479000</v>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G12" t="n">
         <v>52.3167</v>
@@ -772,8 +794,10 @@
       <c r="E13" t="n">
         <v>168</v>
       </c>
-      <c r="F13" t="n">
-        <v>1585650479000</v>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G13" t="n">
         <v>38.9637</v>
@@ -803,8 +827,10 @@
       <c r="E14" t="n">
         <v>2</v>
       </c>
-      <c r="F14" t="n">
-        <v>1585650479000</v>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G14" t="n">
         <v>47.5162</v>
@@ -834,8 +860,10 @@
       <c r="E15" t="n">
         <v>97</v>
       </c>
-      <c r="F15" t="n">
-        <v>1585650479000</v>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G15" t="n">
         <v>35.907757</v>
@@ -865,8 +893,10 @@
       <c r="E16" t="n">
         <v>3</v>
       </c>
-      <c r="F16" t="n">
-        <v>1585650816000</v>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:33:36</t>
+        </is>
       </c>
       <c r="G16" t="n">
         <v>60.001</v>
@@ -896,8 +926,10 @@
       <c r="E17" t="n">
         <v>139</v>
       </c>
-      <c r="F17" t="n">
-        <v>1585650479000</v>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G17" t="n">
         <v>39.3999</v>
@@ -927,8 +959,10 @@
       <c r="E18" t="n">
         <v>91</v>
       </c>
-      <c r="F18" t="n">
-        <v>1585650479000</v>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G18" t="n">
         <v>31.046051</v>
@@ -958,8 +992,10 @@
       <c r="E19" t="n">
         <v>40</v>
       </c>
-      <c r="F19" t="n">
-        <v>1585650479000</v>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G19" t="n">
         <v>-14.235</v>
@@ -989,8 +1025,10 @@
       <c r="E20" t="n">
         <v>1</v>
       </c>
-      <c r="F20" t="n">
-        <v>1585650831000</v>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:33:51</t>
+        </is>
       </c>
       <c r="G20" t="n">
         <v>-25</v>
@@ -1020,8 +1058,10 @@
       <c r="E21" t="n">
         <v>13</v>
       </c>
-      <c r="F21" t="n">
-        <v>1585650479000</v>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G21" t="n">
         <v>60.472</v>
@@ -1051,8 +1091,10 @@
       <c r="E22" t="n">
         <v>15</v>
       </c>
-      <c r="F22" t="n">
-        <v>1585650479000</v>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G22" t="n">
         <v>60.1282</v>
@@ -1082,8 +1124,10 @@
       <c r="E23" t="n">
         <v>59</v>
       </c>
-      <c r="F23" t="n">
-        <v>1585650479000</v>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G23" t="n">
         <v>49.8175</v>
@@ -1113,8 +1157,10 @@
       <c r="E24" t="n">
         <v>5</v>
       </c>
-      <c r="F24" t="n">
-        <v>1585650479000</v>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G24" t="n">
         <v>56</v>
@@ -1144,8 +1190,10 @@
       <c r="E25" t="n">
         <v>10</v>
       </c>
-      <c r="F25" t="n">
-        <v>1585650479000</v>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G25" t="n">
         <v>53.1424</v>
@@ -1175,8 +1223,10 @@
       <c r="E26" t="n">
         <v>111</v>
       </c>
-      <c r="F26" t="n">
-        <v>1585650479000</v>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G26" t="n">
         <v>4.210483999999999</v>
@@ -1206,8 +1256,10 @@
       <c r="E27" t="n">
         <v>50</v>
       </c>
-      <c r="F27" t="n">
-        <v>1585650479000</v>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G27" t="n">
         <v>-35.6751</v>
@@ -1237,8 +1289,10 @@
       <c r="E28" t="n">
         <v>14</v>
       </c>
-      <c r="F28" t="n">
-        <v>1585650479000</v>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G28" t="n">
         <v>61.52399999999999</v>
@@ -1268,8 +1322,10 @@
       <c r="E29" t="n">
         <v>141</v>
       </c>
-      <c r="F29" t="n">
-        <v>1585650479000</v>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G29" t="n">
         <v>45.9432</v>
@@ -1299,8 +1355,10 @@
       <c r="E30" t="n">
         <v>138</v>
       </c>
-      <c r="F30" t="n">
-        <v>1585650479000</v>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G30" t="n">
         <v>51.9194</v>
@@ -1330,8 +1388,10 @@
       <c r="E31" t="n">
         <v>137</v>
       </c>
-      <c r="F31" t="n">
-        <v>1585650479000</v>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G31" t="n">
         <v>12.879721</v>
@@ -1361,8 +1421,10 @@
       <c r="E32" t="n">
         <v>108</v>
       </c>
-      <c r="F32" t="n">
-        <v>1585650479000</v>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G32" t="n">
         <v>49.8153</v>
@@ -1392,8 +1454,10 @@
       <c r="E33" t="n">
         <v>64</v>
       </c>
-      <c r="F33" t="n">
-        <v>1585650479000</v>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G33" t="n">
         <v>-1.8312</v>
@@ -1423,8 +1487,10 @@
       <c r="E34" t="n">
         <v>93</v>
       </c>
-      <c r="F34" t="n">
-        <v>1585650479000</v>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G34" t="n">
         <v>36.204824</v>
@@ -1454,8 +1520,10 @@
       <c r="E35" t="n">
         <v>132</v>
       </c>
-      <c r="F35" t="n">
-        <v>1585650479000</v>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G35" t="n">
         <v>30.3753</v>
@@ -1485,8 +1553,10 @@
       <c r="E36" t="n">
         <v>163</v>
       </c>
-      <c r="F36" t="n">
-        <v>1585650479000</v>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G36" t="n">
         <v>15.870032</v>
@@ -1516,8 +1586,10 @@
       <c r="E37" t="n">
         <v>88</v>
       </c>
-      <c r="F37" t="n">
-        <v>1585650479000</v>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G37" t="n">
         <v>-0.7893</v>
@@ -1547,8 +1619,10 @@
       <c r="E38" t="n">
         <v>147</v>
       </c>
-      <c r="F38" t="n">
-        <v>1585650479000</v>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G38" t="n">
         <v>23.885942</v>
@@ -1578,8 +1652,10 @@
       <c r="E39" t="n">
         <v>6</v>
       </c>
-      <c r="F39" t="n">
-        <v>1585650479000</v>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G39" t="n">
         <v>61.9241</v>
@@ -1609,8 +1685,10 @@
       <c r="E40" t="n">
         <v>155</v>
       </c>
-      <c r="F40" t="n">
-        <v>1585650479000</v>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G40" t="n">
         <v>-30.5595</v>
@@ -1640,8 +1718,10 @@
       <c r="E41" t="n">
         <v>87</v>
       </c>
-      <c r="F41" t="n">
-        <v>1585650479000</v>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G41" t="n">
         <v>20.593684</v>
@@ -1671,8 +1751,10 @@
       <c r="E42" t="n">
         <v>77</v>
       </c>
-      <c r="F42" t="n">
-        <v>1585650479000</v>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G42" t="n">
         <v>39.0742</v>
@@ -1702,8 +1784,10 @@
       <c r="E43" t="n">
         <v>117</v>
       </c>
-      <c r="F43" t="n">
-        <v>1585650479000</v>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G43" t="n">
         <v>23.6345</v>
@@ -1733,8 +1817,10 @@
       <c r="E44" t="n">
         <v>9</v>
       </c>
-      <c r="F44" t="n">
-        <v>1585650479000</v>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G44" t="n">
         <v>64.9631</v>
@@ -1764,8 +1850,10 @@
       <c r="E45" t="n">
         <v>133</v>
       </c>
-      <c r="F45" t="n">
-        <v>1585650479000</v>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G45" t="n">
         <v>8.538</v>
@@ -1795,8 +1883,10 @@
       <c r="E46" t="n">
         <v>25</v>
       </c>
-      <c r="F46" t="n">
-        <v>1585650479000</v>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G46" t="n">
         <v>-38.4161</v>
@@ -1826,8 +1916,10 @@
       <c r="E47" t="n">
         <v>136</v>
       </c>
-      <c r="F47" t="n">
-        <v>1585650479000</v>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G47" t="n">
         <v>-9.19</v>
@@ -1857,8 +1949,10 @@
       <c r="E48" t="n">
         <v>63</v>
       </c>
-      <c r="F48" t="n">
-        <v>1585650479000</v>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G48" t="n">
         <v>18.7357</v>
@@ -1888,8 +1982,10 @@
       <c r="E49" t="n">
         <v>151</v>
       </c>
-      <c r="F49" t="n">
-        <v>1585650479000</v>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G49" t="n">
         <v>1.2833</v>
@@ -1919,8 +2015,10 @@
       <c r="E50" t="n">
         <v>153</v>
       </c>
-      <c r="F50" t="n">
-        <v>1585650479000</v>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G50" t="n">
         <v>46.1512</v>
@@ -1950,8 +2048,10 @@
       <c r="E51" t="n">
         <v>51</v>
       </c>
-      <c r="F51" t="n">
-        <v>1585650479000</v>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G51" t="n">
         <v>4.5709</v>
@@ -1981,8 +2081,10 @@
       <c r="E52" t="n">
         <v>56</v>
       </c>
-      <c r="F52" t="n">
-        <v>1585650479000</v>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G52" t="n">
         <v>45.1</v>
@@ -2012,8 +2114,10 @@
       <c r="E53" t="n">
         <v>149</v>
       </c>
-      <c r="F53" t="n">
-        <v>1585650479000</v>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G53" t="n">
         <v>44.0165</v>
@@ -2043,8 +2147,10 @@
       <c r="E54" t="n">
         <v>69</v>
       </c>
-      <c r="F54" t="n">
-        <v>1585650479000</v>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G54" t="n">
         <v>58.5953</v>
@@ -2074,8 +2180,10 @@
       <c r="E55" t="n">
         <v>60</v>
       </c>
-      <c r="F55" t="n">
-        <v>1585650479000</v>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G55" t="n">
         <v>0</v>
@@ -2105,8 +2213,10 @@
       <c r="E56" t="n">
         <v>140</v>
       </c>
-      <c r="F56" t="n">
-        <v>1585650479000</v>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G56" t="n">
         <v>25.3548</v>
@@ -2136,8 +2246,10 @@
       <c r="E57" t="n">
         <v>65</v>
       </c>
-      <c r="F57" t="n">
-        <v>1585650479000</v>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G57" t="n">
         <v>26.820553</v>
@@ -2167,8 +2279,10 @@
       <c r="E58" t="n">
         <v>126</v>
       </c>
-      <c r="F58" t="n">
-        <v>1585650479000</v>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G58" t="n">
         <v>-40.9006</v>
@@ -2198,8 +2312,10 @@
       <c r="E59" t="n">
         <v>90</v>
       </c>
-      <c r="F59" t="n">
-        <v>1585650479000</v>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G59" t="n">
         <v>33.223191</v>
@@ -2229,8 +2345,10 @@
       <c r="E60" t="n">
         <v>171</v>
       </c>
-      <c r="F60" t="n">
-        <v>1585650479000</v>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G60" t="n">
         <v>23.424076</v>
@@ -2260,8 +2378,10 @@
       <c r="E61" t="n">
         <v>21</v>
       </c>
-      <c r="F61" t="n">
-        <v>1585650479000</v>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G61" t="n">
         <v>28.0339</v>
@@ -2291,8 +2411,10 @@
       <c r="E62" t="n">
         <v>122</v>
       </c>
-      <c r="F62" t="n">
-        <v>1585650479000</v>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G62" t="n">
         <v>31.7917</v>
@@ -2322,8 +2444,10 @@
       <c r="E63" t="n">
         <v>170</v>
       </c>
-      <c r="F63" t="n">
-        <v>1585650479000</v>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G63" t="n">
         <v>48.3794</v>
@@ -2353,8 +2477,10 @@
       <c r="E64" t="n">
         <v>107</v>
       </c>
-      <c r="F64" t="n">
-        <v>1585650479000</v>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G64" t="n">
         <v>55.1694</v>
@@ -2384,8 +2510,10 @@
       <c r="E65" t="n">
         <v>26</v>
       </c>
-      <c r="F65" t="n">
-        <v>1585650479000</v>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G65" t="n">
         <v>40.0691</v>
@@ -2415,8 +2543,10 @@
       <c r="E66" t="n">
         <v>29</v>
       </c>
-      <c r="F66" t="n">
-        <v>1585650479000</v>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G66" t="n">
         <v>26.0275</v>
@@ -2446,8 +2576,10 @@
       <c r="E67" t="n">
         <v>86</v>
       </c>
-      <c r="F67" t="n">
-        <v>1585650479000</v>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G67" t="n">
         <v>47.1625</v>
@@ -2477,8 +2609,10 @@
       <c r="E68" t="n">
         <v>103</v>
       </c>
-      <c r="F68" t="n">
-        <v>1585650479000</v>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G68" t="n">
         <v>33.8547</v>
@@ -2508,8 +2642,10 @@
       <c r="E69" t="n">
         <v>38</v>
       </c>
-      <c r="F69" t="n">
-        <v>1585650479000</v>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G69" t="n">
         <v>43.9159</v>
@@ -2539,8 +2675,10 @@
       <c r="E70" t="n">
         <v>102</v>
       </c>
-      <c r="F70" t="n">
-        <v>1585650479000</v>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G70" t="n">
         <v>56.8796</v>
@@ -2570,8 +2708,10 @@
       <c r="E71" t="n">
         <v>42</v>
       </c>
-      <c r="F71" t="n">
-        <v>1585650479000</v>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G71" t="n">
         <v>42.7339</v>
@@ -2601,8 +2741,10 @@
       <c r="E72" t="n">
         <v>22</v>
       </c>
-      <c r="F72" t="n">
-        <v>1585650479000</v>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G72" t="n">
         <v>42.5063</v>
@@ -2632,8 +2774,10 @@
       <c r="E73" t="n">
         <v>152</v>
       </c>
-      <c r="F73" t="n">
-        <v>1585650479000</v>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G73" t="n">
         <v>48.669</v>
@@ -2663,8 +2807,10 @@
       <c r="E74" t="n">
         <v>167</v>
       </c>
-      <c r="F74" t="n">
-        <v>1585650479000</v>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G74" t="n">
         <v>33.886917</v>
@@ -2694,8 +2840,10 @@
       <c r="E75" t="n">
         <v>95</v>
       </c>
-      <c r="F75" t="n">
-        <v>1585650479000</v>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G75" t="n">
         <v>48.0196</v>
@@ -2725,8 +2873,10 @@
       <c r="E76" t="n">
         <v>54</v>
       </c>
-      <c r="F76" t="n">
-        <v>1585650479000</v>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G76" t="n">
         <v>9.748900000000001</v>
@@ -2756,8 +2906,10 @@
       <c r="E77" t="n">
         <v>161</v>
       </c>
-      <c r="F77" t="n">
-        <v>1585639619000</v>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>2020-03-31 07:26:59</t>
+        </is>
       </c>
       <c r="G77" t="n">
         <v>23.7</v>
@@ -2787,8 +2939,10 @@
       <c r="E78" t="n">
         <v>172</v>
       </c>
-      <c r="F78" t="n">
-        <v>1585650479000</v>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G78" t="n">
         <v>-32.5228</v>
@@ -2818,8 +2972,10 @@
       <c r="E79" t="n">
         <v>118</v>
       </c>
-      <c r="F79" t="n">
-        <v>1585650479000</v>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G79" t="n">
         <v>47.4116</v>
@@ -2849,8 +3005,10 @@
       <c r="E80" t="n">
         <v>99</v>
       </c>
-      <c r="F80" t="n">
-        <v>1585650479000</v>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G80" t="n">
         <v>29.31166</v>
@@ -2880,8 +3038,10 @@
       <c r="E81" t="n">
         <v>130</v>
       </c>
-      <c r="F81" t="n">
-        <v>1585650479000</v>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G81" t="n">
         <v>41.6086</v>
@@ -2911,8 +3071,10 @@
       <c r="E82" t="n">
         <v>27</v>
       </c>
-      <c r="F82" t="n">
-        <v>1585650479000</v>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G82" t="n">
         <v>40.1431</v>
@@ -2942,8 +3104,10 @@
       <c r="E83" t="n">
         <v>94</v>
       </c>
-      <c r="F83" t="n">
-        <v>1585650479000</v>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G83" t="n">
         <v>31.24</v>
@@ -2973,8 +3137,10 @@
       <c r="E84" t="n">
         <v>43</v>
       </c>
-      <c r="F84" t="n">
-        <v>1585650479000</v>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G84" t="n">
         <v>12.2383</v>
@@ -3004,8 +3170,10 @@
       <c r="E85" t="n">
         <v>20</v>
       </c>
-      <c r="F85" t="n">
-        <v>1585650479000</v>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G85" t="n">
         <v>41.1533</v>
@@ -3035,8 +3203,10 @@
       <c r="E86" t="n">
         <v>58</v>
       </c>
-      <c r="F86" t="n">
-        <v>1585650479000</v>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G86" t="n">
         <v>35.1264</v>
@@ -3066,8 +3236,10 @@
       <c r="E87" t="n">
         <v>146</v>
       </c>
-      <c r="F87" t="n">
-        <v>1585650479000</v>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G87" t="n">
         <v>43.9424</v>
@@ -3097,8 +3269,10 @@
       <c r="E88" t="n">
         <v>175</v>
       </c>
-      <c r="F88" t="n">
-        <v>1585650479000</v>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G88" t="n">
         <v>14.058324</v>
@@ -3128,8 +3302,10 @@
       <c r="E89" t="n">
         <v>47</v>
       </c>
-      <c r="F89" t="n">
-        <v>1585650479000</v>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G89" t="n">
         <v>3.848</v>
@@ -3159,8 +3335,10 @@
       <c r="E90" t="n">
         <v>131</v>
       </c>
-      <c r="F90" t="n">
-        <v>1585650479000</v>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G90" t="n">
         <v>21.512583</v>
@@ -3190,8 +3368,10 @@
       <c r="E91" t="n">
         <v>148</v>
       </c>
-      <c r="F91" t="n">
-        <v>1585650479000</v>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G91" t="n">
         <v>14.4974</v>
@@ -3221,8 +3401,10 @@
       <c r="E92" t="n">
         <v>19</v>
       </c>
-      <c r="F92" t="n">
-        <v>1585650479000</v>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G92" t="n">
         <v>33.93911</v>
@@ -3252,8 +3434,10 @@
       <c r="E93" t="n">
         <v>57</v>
       </c>
-      <c r="F93" t="n">
-        <v>1585650479000</v>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G93" t="n">
         <v>21.521757</v>
@@ -3283,8 +3467,10 @@
       <c r="E94" t="n">
         <v>55</v>
       </c>
-      <c r="F94" t="n">
-        <v>1585650479000</v>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G94" t="n">
         <v>7.54</v>
@@ -3314,8 +3500,10 @@
       <c r="E95" t="n">
         <v>173</v>
       </c>
-      <c r="F95" t="n">
-        <v>1585650479000</v>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G95" t="n">
         <v>41.377491</v>
@@ -3345,8 +3533,10 @@
       <c r="E96" t="n">
         <v>114</v>
       </c>
-      <c r="F96" t="n">
-        <v>1585650479000</v>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G96" t="n">
         <v>35.9375</v>
@@ -3376,8 +3566,10 @@
       <c r="E97" t="n">
         <v>32</v>
       </c>
-      <c r="F97" t="n">
-        <v>1585650479000</v>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G97" t="n">
         <v>53.7098</v>
@@ -3407,8 +3599,10 @@
       <c r="E98" t="n">
         <v>76</v>
       </c>
-      <c r="F98" t="n">
-        <v>1585650479000</v>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G98" t="n">
         <v>7.9465</v>
@@ -3438,8 +3632,10 @@
       <c r="E99" t="n">
         <v>116</v>
       </c>
-      <c r="F99" t="n">
-        <v>1585650479000</v>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G99" t="n">
         <v>-20.348404</v>
@@ -3469,8 +3665,10 @@
       <c r="E100" t="n">
         <v>85</v>
       </c>
-      <c r="F100" t="n">
-        <v>1585650479000</v>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G100" t="n">
         <v>15.2</v>
@@ -3500,8 +3698,10 @@
       <c r="E101" t="n">
         <v>174</v>
       </c>
-      <c r="F101" t="n">
-        <v>1585650479000</v>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G101" t="n">
         <v>6.4238</v>
@@ -3531,8 +3731,10 @@
       <c r="E102" t="n">
         <v>129</v>
       </c>
-      <c r="F102" t="n">
-        <v>1585650479000</v>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G102" t="n">
         <v>9.082000000000001</v>
@@ -3562,8 +3764,10 @@
       <c r="E103" t="n">
         <v>41</v>
       </c>
-      <c r="F103" t="n">
-        <v>1585650479000</v>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G103" t="n">
         <v>4.5353</v>
@@ -3593,8 +3797,10 @@
       <c r="E104" t="n">
         <v>157</v>
       </c>
-      <c r="F104" t="n">
-        <v>1585650479000</v>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G104" t="n">
         <v>7.873054</v>
@@ -3624,8 +3830,10 @@
       <c r="E105" t="n">
         <v>176</v>
       </c>
-      <c r="F105" t="n">
-        <v>1585650479000</v>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G105" t="n">
         <v>31.9522</v>
@@ -3655,8 +3863,10 @@
       <c r="E106" t="n">
         <v>75</v>
       </c>
-      <c r="F106" t="n">
-        <v>1585650479000</v>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G106" t="n">
         <v>42.3154</v>
@@ -3686,8 +3896,10 @@
       <c r="E107" t="n">
         <v>46</v>
       </c>
-      <c r="F107" t="n">
-        <v>1585650479000</v>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G107" t="n">
         <v>11.55</v>
@@ -3717,8 +3929,10 @@
       <c r="E108" t="n">
         <v>37</v>
       </c>
-      <c r="F108" t="n">
-        <v>1585650479000</v>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G108" t="n">
         <v>-16.2902</v>
@@ -3748,8 +3962,10 @@
       <c r="E109" t="n">
         <v>100</v>
       </c>
-      <c r="F109" t="n">
-        <v>1585650479000</v>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G109" t="n">
         <v>41.20438</v>
@@ -3779,8 +3995,10 @@
       <c r="E110" t="n">
         <v>98</v>
       </c>
-      <c r="F110" t="n">
-        <v>1585650479000</v>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G110" t="n">
         <v>42.602636</v>
@@ -3810,8 +4028,10 @@
       <c r="E111" t="n">
         <v>121</v>
       </c>
-      <c r="F111" t="n">
-        <v>1585650479000</v>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G111" t="n">
         <v>42.70867800000001</v>
@@ -3841,8 +4061,10 @@
       <c r="E112" t="n">
         <v>53</v>
       </c>
-      <c r="F112" t="n">
-        <v>1585650479000</v>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G112" t="n">
         <v>-4.322447</v>
@@ -3872,8 +4094,10 @@
       <c r="E113" t="n">
         <v>166</v>
       </c>
-      <c r="F113" t="n">
-        <v>1585650479000</v>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G113" t="n">
         <v>10.6918</v>
@@ -3903,8 +4127,10 @@
       <c r="E114" t="n">
         <v>142</v>
       </c>
-      <c r="F114" t="n">
-        <v>1585650479000</v>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G114" t="n">
         <v>-1.9403</v>
@@ -3934,8 +4160,10 @@
       <c r="E115" t="n">
         <v>135</v>
       </c>
-      <c r="F115" t="n">
-        <v>1585650479000</v>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G115" t="n">
         <v>-23.4425</v>
@@ -3965,8 +4193,10 @@
       <c r="E116" t="n">
         <v>106</v>
       </c>
-      <c r="F116" t="n">
-        <v>1585650479000</v>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G116" t="n">
         <v>47.14</v>
@@ -3996,8 +4226,10 @@
       <c r="E117" t="n">
         <v>30</v>
       </c>
-      <c r="F117" t="n">
-        <v>1585650479000</v>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G117" t="n">
         <v>23.685</v>
@@ -4027,8 +4259,10 @@
       <c r="E118" t="n">
         <v>96</v>
       </c>
-      <c r="F118" t="n">
-        <v>1585650479000</v>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G118" t="n">
         <v>-0.0236</v>
@@ -4058,8 +4292,10 @@
       <c r="E119" t="n">
         <v>119</v>
       </c>
-      <c r="F119" t="n">
-        <v>1585650479000</v>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G119" t="n">
         <v>43.7333</v>
@@ -4089,8 +4325,10 @@
       <c r="E120" t="n">
         <v>110</v>
       </c>
-      <c r="F120" t="n">
-        <v>1585650479000</v>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G120" t="n">
         <v>-18.766947</v>
@@ -4120,8 +4358,10 @@
       <c r="E121" t="n">
         <v>79</v>
       </c>
-      <c r="F121" t="n">
-        <v>1585650479000</v>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G121" t="n">
         <v>15.7835</v>
@@ -4151,8 +4391,10 @@
       <c r="E122" t="n">
         <v>92</v>
       </c>
-      <c r="F122" t="n">
-        <v>1585650479000</v>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G122" t="n">
         <v>18.1096</v>
@@ -4182,8 +4424,10 @@
       <c r="E123" t="n">
         <v>177</v>
       </c>
-      <c r="F123" t="n">
-        <v>1585650479000</v>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G123" t="n">
         <v>-13.133897</v>
@@ -4213,8 +4457,10 @@
       <c r="E124" t="n">
         <v>31</v>
       </c>
-      <c r="F124" t="n">
-        <v>1585650479000</v>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G124" t="n">
         <v>13.1939</v>
@@ -4244,8 +4490,10 @@
       <c r="E125" t="n">
         <v>169</v>
       </c>
-      <c r="F125" t="n">
-        <v>1585650479000</v>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G125" t="n">
         <v>1.373333</v>
@@ -4275,8 +4523,10 @@
       <c r="E126" t="n">
         <v>66</v>
       </c>
-      <c r="F126" t="n">
-        <v>1585650479000</v>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G126" t="n">
         <v>13.7942</v>
@@ -4306,8 +4556,10 @@
       <c r="E127" t="n">
         <v>165</v>
       </c>
-      <c r="F127" t="n">
-        <v>1585650479000</v>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G127" t="n">
         <v>8.6195</v>
@@ -4337,8 +4589,10 @@
       <c r="E128" t="n">
         <v>128</v>
       </c>
-      <c r="F128" t="n">
-        <v>1585650479000</v>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G128" t="n">
         <v>17.607789</v>
@@ -4368,8 +4622,10 @@
       <c r="E129" t="n">
         <v>71</v>
       </c>
-      <c r="F129" t="n">
-        <v>1585650479000</v>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G129" t="n">
         <v>9.145</v>
@@ -4399,8 +4655,10 @@
       <c r="E130" t="n">
         <v>113</v>
       </c>
-      <c r="F130" t="n">
-        <v>1585650479000</v>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G130" t="n">
         <v>17.570692</v>
@@ -4430,8 +4688,10 @@
       <c r="E131" t="n">
         <v>80</v>
       </c>
-      <c r="F131" t="n">
-        <v>1585650479000</v>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G131" t="n">
         <v>9.945600000000001</v>
@@ -4461,8 +4721,10 @@
       <c r="E132" t="n">
         <v>52</v>
       </c>
-      <c r="F132" t="n">
-        <v>1585650479000</v>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G132" t="n">
         <v>-4.2634</v>
@@ -4492,8 +4754,10 @@
       <c r="E133" t="n">
         <v>162</v>
       </c>
-      <c r="F133" t="n">
-        <v>1585650479000</v>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G133" t="n">
         <v>-6.369028</v>
@@ -4523,8 +4787,10 @@
       <c r="E134" t="n">
         <v>61</v>
       </c>
-      <c r="F134" t="n">
-        <v>1585650479000</v>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G134" t="n">
         <v>11.8251</v>
@@ -4554,8 +4820,10 @@
       <c r="E135" t="n">
         <v>112</v>
       </c>
-      <c r="F135" t="n">
-        <v>1585650479000</v>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G135" t="n">
         <v>3.2028</v>
@@ -4585,8 +4853,10 @@
       <c r="E136" t="n">
         <v>73</v>
       </c>
-      <c r="F136" t="n">
-        <v>1585650479000</v>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G136" t="n">
         <v>-0.8037</v>
@@ -4616,8 +4886,10 @@
       <c r="E137" t="n">
         <v>68</v>
       </c>
-      <c r="F137" t="n">
-        <v>1585650479000</v>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G137" t="n">
         <v>15.1794</v>
@@ -4647,8 +4919,10 @@
       <c r="E138" t="n">
         <v>83</v>
       </c>
-      <c r="F138" t="n">
-        <v>1585650479000</v>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G138" t="n">
         <v>18.9712</v>
@@ -4678,8 +4952,10 @@
       <c r="E139" t="n">
         <v>28</v>
       </c>
-      <c r="F139" t="n">
-        <v>1585650479000</v>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G139" t="n">
         <v>25.025885</v>
@@ -4709,8 +4985,10 @@
       <c r="E140" t="n">
         <v>44</v>
       </c>
-      <c r="F140" t="n">
-        <v>1585650479000</v>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G140" t="n">
         <v>21.9162</v>
@@ -4740,8 +5018,10 @@
       <c r="E141" t="n">
         <v>62</v>
       </c>
-      <c r="F141" t="n">
-        <v>1585650479000</v>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G141" t="n">
         <v>15.415</v>
@@ -4771,8 +5051,10 @@
       <c r="E142" t="n">
         <v>67</v>
       </c>
-      <c r="F142" t="n">
-        <v>1585650479000</v>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G142" t="n">
         <v>1.6508</v>
@@ -4802,8 +5084,10 @@
       <c r="E143" t="n">
         <v>120</v>
       </c>
-      <c r="F143" t="n">
-        <v>1585650479000</v>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G143" t="n">
         <v>46.8625</v>
@@ -4833,8 +5117,10 @@
       <c r="E144" t="n">
         <v>124</v>
       </c>
-      <c r="F144" t="n">
-        <v>1585650479000</v>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G144" t="n">
         <v>-22.9576</v>
@@ -4864,8 +5150,10 @@
       <c r="E145" t="n">
         <v>150</v>
       </c>
-      <c r="F145" t="n">
-        <v>1585650479000</v>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G145" t="n">
         <v>-4.6796</v>
@@ -4895,8 +5183,10 @@
       <c r="E146" t="n">
         <v>160</v>
       </c>
-      <c r="F146" t="n">
-        <v>1585650479000</v>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G146" t="n">
         <v>34.802075</v>
@@ -4926,8 +5216,10 @@
       <c r="E147" t="n">
         <v>70</v>
       </c>
-      <c r="F147" t="n">
-        <v>1585650479000</v>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G147" t="n">
         <v>-26.5225</v>
@@ -4957,8 +5249,10 @@
       <c r="E148" t="n">
         <v>78</v>
       </c>
-      <c r="F148" t="n">
-        <v>1585650479000</v>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G148" t="n">
         <v>12.1165</v>
@@ -4988,8 +5282,10 @@
       <c r="E149" t="n">
         <v>101</v>
       </c>
-      <c r="F149" t="n">
-        <v>1585650479000</v>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G149" t="n">
         <v>19.85627</v>
@@ -5019,8 +5315,10 @@
       <c r="E150" t="n">
         <v>144</v>
       </c>
-      <c r="F150" t="n">
-        <v>1585650479000</v>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G150" t="n">
         <v>13.9094</v>
@@ -5050,8 +5348,10 @@
       <c r="E151" t="n">
         <v>81</v>
       </c>
-      <c r="F151" t="n">
-        <v>1585650479000</v>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G151" t="n">
         <v>11.8037</v>
@@ -5081,8 +5381,10 @@
       <c r="E152" t="n">
         <v>82</v>
       </c>
-      <c r="F152" t="n">
-        <v>1585650479000</v>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G152" t="n">
         <v>4.860416000000001</v>
@@ -5112,8 +5414,10 @@
       <c r="E153" t="n">
         <v>105</v>
       </c>
-      <c r="F153" t="n">
-        <v>1585650479000</v>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G153" t="n">
         <v>26.3351</v>
@@ -5143,8 +5447,10 @@
       <c r="E154" t="n">
         <v>123</v>
       </c>
-      <c r="F154" t="n">
-        <v>1585650479000</v>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G154" t="n">
         <v>-18.665695</v>
@@ -5174,8 +5480,10 @@
       <c r="E155" t="n">
         <v>159</v>
       </c>
-      <c r="F155" t="n">
-        <v>1585650479000</v>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G155" t="n">
         <v>3.9193</v>
@@ -5205,8 +5513,10 @@
       <c r="E156" t="n">
         <v>178</v>
       </c>
-      <c r="F156" t="n">
-        <v>1585650479000</v>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G156" t="n">
         <v>-19.015438</v>
@@ -5236,8 +5546,10 @@
       <c r="E157" t="n">
         <v>23</v>
       </c>
-      <c r="F157" t="n">
-        <v>1585650479000</v>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G157" t="n">
         <v>-11.2027</v>
@@ -5267,8 +5579,10 @@
       <c r="E158" t="n">
         <v>24</v>
       </c>
-      <c r="F158" t="n">
-        <v>1585650479000</v>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G158" t="n">
         <v>17.0608</v>
@@ -5298,8 +5612,10 @@
       <c r="E159" t="n">
         <v>49</v>
       </c>
-      <c r="F159" t="n">
-        <v>1585650479000</v>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G159" t="n">
         <v>15.4542</v>
@@ -5329,8 +5645,10 @@
       <c r="E160" t="n">
         <v>143</v>
       </c>
-      <c r="F160" t="n">
-        <v>1585650479000</v>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G160" t="n">
         <v>17.357822</v>
@@ -5360,8 +5678,10 @@
       <c r="E161" t="n">
         <v>158</v>
       </c>
-      <c r="F161" t="n">
-        <v>1585650479000</v>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G161" t="n">
         <v>12.8628</v>
@@ -5391,8 +5711,10 @@
       <c r="E162" t="n">
         <v>35</v>
       </c>
-      <c r="F162" t="n">
-        <v>1585650479000</v>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G162" t="n">
         <v>9.307700000000001</v>
@@ -5422,8 +5744,10 @@
       <c r="E163" t="n">
         <v>45</v>
       </c>
-      <c r="F163" t="n">
-        <v>1585650479000</v>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G163" t="n">
         <v>16.5388</v>
@@ -5453,8 +5777,10 @@
       <c r="E164" t="n">
         <v>84</v>
       </c>
-      <c r="F164" t="n">
-        <v>1585650479000</v>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G164" t="n">
         <v>41.9029</v>
@@ -5484,8 +5810,10 @@
       <c r="E165" t="n">
         <v>115</v>
       </c>
-      <c r="F165" t="n">
-        <v>1585650479000</v>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G165" t="n">
         <v>21.0079</v>
@@ -5515,8 +5843,10 @@
       <c r="E166" t="n">
         <v>72</v>
       </c>
-      <c r="F166" t="n">
-        <v>1585650479000</v>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G166" t="n">
         <v>-17.7134</v>
@@ -5546,8 +5876,10 @@
       <c r="E167" t="n">
         <v>125</v>
       </c>
-      <c r="F167" t="n">
-        <v>1585650479000</v>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G167" t="n">
         <v>28.1667</v>
@@ -5577,8 +5909,10 @@
       <c r="E168" t="n">
         <v>36</v>
       </c>
-      <c r="F168" t="n">
-        <v>1585650479000</v>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G168" t="n">
         <v>27.5142</v>
@@ -5608,8 +5942,10 @@
       <c r="E169" t="n">
         <v>74</v>
       </c>
-      <c r="F169" t="n">
-        <v>1585650479000</v>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G169" t="n">
         <v>13.4432</v>
@@ -5639,8 +5975,10 @@
       <c r="E170" t="n">
         <v>127</v>
       </c>
-      <c r="F170" t="n">
-        <v>1585650479000</v>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G170" t="n">
         <v>12.865416</v>
@@ -5670,8 +6008,10 @@
       <c r="E171" t="n">
         <v>34</v>
       </c>
-      <c r="F171" t="n">
-        <v>1585650479000</v>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G171" t="n">
         <v>17.1899</v>
@@ -5701,8 +6041,10 @@
       <c r="E172" t="n">
         <v>39</v>
       </c>
-      <c r="F172" t="n">
-        <v>1585650479000</v>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G172" t="n">
         <v>-22.3285</v>
@@ -5732,8 +6074,10 @@
       <c r="E173" t="n">
         <v>48</v>
       </c>
-      <c r="F173" t="n">
-        <v>1585650479000</v>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G173" t="n">
         <v>6.6111</v>
@@ -5763,8 +6107,10 @@
       <c r="E174" t="n">
         <v>104</v>
       </c>
-      <c r="F174" t="n">
-        <v>1585650479000</v>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G174" t="n">
         <v>6.428055000000001</v>
@@ -5794,8 +6140,10 @@
       <c r="E175" t="n">
         <v>154</v>
       </c>
-      <c r="F175" t="n">
-        <v>1585650479000</v>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G175" t="n">
         <v>5.152149</v>
@@ -5825,8 +6173,10 @@
       <c r="E176" t="n">
         <v>109</v>
       </c>
-      <c r="F176" t="n">
-        <v>1585650479000</v>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G176" t="n">
         <v>0</v>
@@ -5856,8 +6206,10 @@
       <c r="E177" t="n">
         <v>134</v>
       </c>
-      <c r="F177" t="n">
-        <v>1585650479000</v>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G177" t="n">
         <v>-6.314993</v>
@@ -5887,8 +6239,10 @@
       <c r="E178" t="n">
         <v>145</v>
       </c>
-      <c r="F178" t="n">
-        <v>1585650479000</v>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G178" t="n">
         <v>12.9843</v>
@@ -5918,8 +6272,10 @@
       <c r="E179" t="n">
         <v>164</v>
       </c>
-      <c r="F179" t="n">
-        <v>1585650479000</v>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>2020-03-31 10:27:59</t>
+        </is>
       </c>
       <c r="G179" t="n">
         <v>-8.874217</v>

</xml_diff>